<commit_message>
Updated working file and variables file
</commit_message>
<xml_diff>
--- a/House_Variables.xlsx
+++ b/House_Variables.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfaupel/Desktop/Projects/Housing_Price_Prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4C62C5A2-A0E0-9441-9349-53A4652612F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80071DCC-4D3E-AB46-BF93-F70AC1917356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2360" yWindow="1400" windowWidth="27640" windowHeight="16940" xr2:uid="{6CC0573A-78B8-8B47-B289-8880F04E05D3}"/>
+    <workbookView xWindow="1440" yWindow="1740" windowWidth="27640" windowHeight="16940" xr2:uid="{6CC0573A-78B8-8B47-B289-8880F04E05D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="111">
   <si>
     <t>Column</t>
   </si>
@@ -755,7 +755,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -794,13 +794,13 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D2" t="s">
         <v>90</v>
@@ -809,21 +809,18 @@
         <v>90</v>
       </c>
       <c r="F2" t="s">
-        <v>86</v>
-      </c>
-      <c r="G2" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D3" t="s">
         <v>90</v>
@@ -832,44 +829,41 @@
         <v>90</v>
       </c>
       <c r="F3" t="s">
-        <v>98</v>
-      </c>
-      <c r="G3" t="s">
-        <v>90</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3</v>
+        <v>95</v>
       </c>
       <c r="C4" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D4" t="s">
         <v>90</v>
       </c>
       <c r="E4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F4" t="s">
-        <v>98</v>
+        <v>102</v>
       </c>
       <c r="G4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>4</v>
+        <v>31</v>
       </c>
       <c r="C5" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
         <v>85</v>
@@ -878,47 +872,47 @@
         <v>90</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E6" t="s">
         <v>90</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="C7" t="s">
         <v>87</v>
       </c>
       <c r="D7" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E7" t="s">
         <v>90</v>
       </c>
       <c r="F7" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G7" t="s">
         <v>90</v>
@@ -926,10 +920,10 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>34</v>
       </c>
       <c r="C8" t="s">
         <v>87</v>
@@ -941,7 +935,7 @@
         <v>90</v>
       </c>
       <c r="F8" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G8" t="s">
         <v>90</v>
@@ -949,13 +943,13 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="C9" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
         <v>90</v>
@@ -964,30 +958,27 @@
         <v>90</v>
       </c>
       <c r="F9" t="s">
-        <v>99</v>
-      </c>
-      <c r="G9" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>9</v>
+        <v>36</v>
       </c>
       <c r="C10" t="s">
         <v>87</v>
       </c>
       <c r="D10" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E10" t="s">
         <v>90</v>
       </c>
       <c r="F10" t="s">
-        <v>99</v>
+        <v>104</v>
       </c>
       <c r="G10" t="s">
         <v>90</v>
@@ -995,13 +986,13 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>10</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D11" t="s">
         <v>90</v>
@@ -1010,18 +1001,18 @@
         <v>90</v>
       </c>
       <c r="F11" t="s">
-        <v>100</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>11</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D12" t="s">
         <v>90</v>
@@ -1030,21 +1021,18 @@
         <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
-      </c>
-      <c r="G12" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>12</v>
+        <v>39</v>
       </c>
       <c r="C13" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D13" t="s">
         <v>90</v>
@@ -1053,21 +1041,18 @@
         <v>90</v>
       </c>
       <c r="F13" t="s">
-        <v>99</v>
-      </c>
-      <c r="G13" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="C14" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D14" t="s">
         <v>90</v>
@@ -1076,18 +1061,18 @@
         <v>90</v>
       </c>
       <c r="F14" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="C15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D15" t="s">
         <v>90</v>
@@ -1096,21 +1081,18 @@
         <v>90</v>
       </c>
       <c r="F15" t="s">
-        <v>99</v>
-      </c>
-      <c r="G15" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="C16" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D16" t="s">
         <v>90</v>
@@ -1119,21 +1101,18 @@
         <v>90</v>
       </c>
       <c r="F16" t="s">
-        <v>99</v>
-      </c>
-      <c r="G16" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>16</v>
+        <v>51</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D17" t="s">
         <v>90</v>
@@ -1142,18 +1121,15 @@
         <v>90</v>
       </c>
       <c r="F17" t="s">
-        <v>98</v>
-      </c>
-      <c r="G17" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="C18" t="s">
         <v>87</v>
@@ -1173,10 +1149,10 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>18</v>
+        <v>3</v>
       </c>
       <c r="C19" t="s">
         <v>87</v>
@@ -1188,15 +1164,18 @@
         <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="G19" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="C20" t="s">
         <v>87</v>
@@ -1208,18 +1187,21 @@
         <v>90</v>
       </c>
       <c r="F20" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="G20" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D21" t="s">
         <v>90</v>
@@ -1228,18 +1210,21 @@
         <v>90</v>
       </c>
       <c r="F21" t="s">
-        <v>102</v>
+        <v>98</v>
+      </c>
+      <c r="G21" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D22" t="s">
         <v>90</v>
@@ -1248,15 +1233,15 @@
         <v>90</v>
       </c>
       <c r="F22" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C23" t="s">
         <v>87</v>
@@ -1273,10 +1258,10 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
         <v>87</v>
@@ -1293,10 +1278,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C25" t="s">
         <v>87</v>
@@ -1313,16 +1298,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C26" t="s">
         <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E26" t="s">
         <v>90</v>
@@ -1333,13 +1318,13 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C27" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D27" t="s">
         <v>85</v>
@@ -1350,19 +1335,22 @@
       <c r="F27" t="s">
         <v>98</v>
       </c>
+      <c r="G27" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C28" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E28" t="s">
         <v>90</v>
@@ -1370,16 +1358,13 @@
       <c r="F28" t="s">
         <v>98</v>
       </c>
-      <c r="G28" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>28</v>
-      </c>
-      <c r="B29" s="1" t="s">
-        <v>28</v>
+        <v>84</v>
+      </c>
+      <c r="B29" t="s">
+        <v>96</v>
       </c>
       <c r="C29" t="s">
         <v>87</v>
@@ -1388,58 +1373,64 @@
         <v>90</v>
       </c>
       <c r="E29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F29" t="s">
-        <v>103</v>
+        <v>98</v>
+      </c>
+      <c r="G29" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>29</v>
+        <v>59</v>
       </c>
       <c r="C30" t="s">
         <v>87</v>
       </c>
       <c r="D30" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E30" t="s">
         <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>103</v>
+        <v>108</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>30</v>
+        <v>60</v>
       </c>
       <c r="C31" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D31" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E31" t="s">
         <v>90</v>
       </c>
       <c r="F31" t="s">
-        <v>98</v>
+        <v>108</v>
+      </c>
+      <c r="G31" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>31</v>
+        <v>61</v>
       </c>
       <c r="C32" t="s">
         <v>87</v>
@@ -1451,58 +1442,55 @@
         <v>90</v>
       </c>
       <c r="F32" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="C33" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E33" t="s">
         <v>90</v>
       </c>
       <c r="F33" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C34" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D34" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E34" t="s">
         <v>90</v>
       </c>
       <c r="F34" t="s">
-        <v>104</v>
-      </c>
-      <c r="G34" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="C35" t="s">
         <v>87</v>
@@ -1514,64 +1502,58 @@
         <v>90</v>
       </c>
       <c r="F35" t="s">
-        <v>104</v>
-      </c>
-      <c r="G35" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="C36" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D36" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E36" t="s">
         <v>90</v>
       </c>
       <c r="F36" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>36</v>
+        <v>18</v>
       </c>
       <c r="C37" t="s">
         <v>87</v>
       </c>
       <c r="D37" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E37" t="s">
         <v>90</v>
       </c>
       <c r="F37" t="s">
-        <v>104</v>
-      </c>
-      <c r="G37" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="C38" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D38" t="s">
         <v>90</v>
@@ -1580,18 +1562,18 @@
         <v>90</v>
       </c>
       <c r="F38" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D39" t="s">
         <v>90</v>
@@ -1600,18 +1582,18 @@
         <v>90</v>
       </c>
       <c r="F39" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>39</v>
+        <v>29</v>
       </c>
       <c r="C40" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D40" t="s">
         <v>90</v>
@@ -1620,15 +1602,15 @@
         <v>90</v>
       </c>
       <c r="F40" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>40</v>
+        <v>54</v>
       </c>
       <c r="C41" t="s">
         <v>87</v>
@@ -1640,15 +1622,15 @@
         <v>90</v>
       </c>
       <c r="F41" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>41</v>
+        <v>56</v>
       </c>
       <c r="C42" t="s">
         <v>87</v>
@@ -1660,18 +1642,18 @@
         <v>90</v>
       </c>
       <c r="F42" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="C43" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D43" t="s">
         <v>90</v>
@@ -1680,35 +1662,35 @@
         <v>90</v>
       </c>
       <c r="F43" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="C44" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D44" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E44" t="s">
         <v>90</v>
       </c>
       <c r="F44" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="C45" t="s">
         <v>88</v>
@@ -1723,12 +1705,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="C46" t="s">
         <v>88</v>
@@ -1743,12 +1725,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="C47" t="s">
         <v>88</v>
@@ -1763,12 +1745,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="C48" t="s">
         <v>88</v>
@@ -1785,10 +1767,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>48</v>
+        <v>55</v>
       </c>
       <c r="C49" t="s">
         <v>88</v>
@@ -1800,18 +1782,18 @@
         <v>90</v>
       </c>
       <c r="F49" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D50" t="s">
         <v>90</v>
@@ -1820,18 +1802,21 @@
         <v>90</v>
       </c>
       <c r="F50" t="s">
-        <v>106</v>
+        <v>86</v>
+      </c>
+      <c r="G50" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>50</v>
+        <v>13</v>
       </c>
       <c r="C51" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D51" t="s">
         <v>90</v>
@@ -1840,55 +1825,61 @@
         <v>90</v>
       </c>
       <c r="F51" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>51</v>
-      </c>
-      <c r="B52" s="1" t="s">
-        <v>51</v>
+        <v>85</v>
+      </c>
+      <c r="B52" t="s">
+        <v>97</v>
       </c>
       <c r="C52" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D52" t="s">
         <v>90</v>
       </c>
       <c r="E52" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F52" t="s">
-        <v>106</v>
+        <v>101</v>
+      </c>
+      <c r="G52" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>52</v>
+        <v>4</v>
       </c>
       <c r="C53" t="s">
         <v>88</v>
       </c>
       <c r="D53" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E53" t="s">
         <v>90</v>
       </c>
       <c r="F53" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="G53" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>53</v>
+        <v>5</v>
       </c>
       <c r="C54" t="s">
         <v>88</v>
@@ -1900,15 +1891,18 @@
         <v>90</v>
       </c>
       <c r="F54" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="G54" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>54</v>
+        <v>6</v>
       </c>
       <c r="C55" t="s">
         <v>87</v>
@@ -1920,35 +1914,41 @@
         <v>90</v>
       </c>
       <c r="F55" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="G55" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="C56" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D56" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E56" t="s">
         <v>90</v>
       </c>
       <c r="F56" t="s">
-        <v>105</v>
+        <v>99</v>
+      </c>
+      <c r="G56" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>56</v>
+        <v>8</v>
       </c>
       <c r="C57" t="s">
         <v>87</v>
@@ -1960,18 +1960,21 @@
         <v>90</v>
       </c>
       <c r="F57" t="s">
-        <v>103</v>
+        <v>99</v>
+      </c>
+      <c r="G57" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>57</v>
+        <v>9</v>
       </c>
       <c r="C58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D58" t="s">
         <v>90</v>
@@ -1980,67 +1983,76 @@
         <v>90</v>
       </c>
       <c r="F58" t="s">
-        <v>107</v>
+        <v>99</v>
+      </c>
+      <c r="G58" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>58</v>
+        <v>11</v>
       </c>
       <c r="C59" t="s">
         <v>87</v>
       </c>
       <c r="D59" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E59" t="s">
         <v>90</v>
       </c>
       <c r="F59" t="s">
-        <v>107</v>
+        <v>99</v>
+      </c>
+      <c r="G59" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>59</v>
+        <v>12</v>
       </c>
       <c r="C60" t="s">
         <v>87</v>
       </c>
       <c r="D60" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E60" t="s">
         <v>90</v>
       </c>
       <c r="F60" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="G60" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="C61" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D61" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E61" t="s">
         <v>90</v>
       </c>
       <c r="F61" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="G61" t="s">
         <v>90</v>
@@ -2048,30 +2060,33 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>61</v>
+        <v>15</v>
       </c>
       <c r="C62" t="s">
         <v>87</v>
       </c>
       <c r="D62" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E62" t="s">
         <v>90</v>
       </c>
       <c r="F62" t="s">
-        <v>108</v>
+        <v>99</v>
+      </c>
+      <c r="G62" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="C63" t="s">
         <v>88</v>
@@ -2083,81 +2098,81 @@
         <v>90</v>
       </c>
       <c r="F63" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C64" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D64" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E64" t="s">
         <v>90</v>
       </c>
       <c r="F64" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C65" t="s">
         <v>87</v>
       </c>
       <c r="D65" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E65" t="s">
         <v>90</v>
       </c>
       <c r="F65" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="C66" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D66" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E66" t="s">
         <v>90</v>
       </c>
       <c r="F66" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>66</v>
+        <v>73</v>
       </c>
       <c r="C67" t="s">
         <v>87</v>
       </c>
       <c r="D67" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E67" t="s">
         <v>90</v>
@@ -2168,30 +2183,30 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C68" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D68" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E68" t="s">
         <v>90</v>
       </c>
       <c r="F68" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C69" t="s">
         <v>88</v>
@@ -2203,15 +2218,15 @@
         <v>90</v>
       </c>
       <c r="F69" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C70" t="s">
         <v>88</v>
@@ -2228,10 +2243,10 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C71" t="s">
         <v>88</v>
@@ -2248,10 +2263,10 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C72" t="s">
         <v>88</v>
@@ -2268,10 +2283,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C73" t="s">
         <v>88</v>
@@ -2283,27 +2298,27 @@
         <v>90</v>
       </c>
       <c r="F73" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C74" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D74" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E74" t="s">
         <v>90</v>
       </c>
       <c r="F74" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
@@ -2328,30 +2343,33 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C76" t="s">
         <v>87</v>
       </c>
       <c r="D76" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E76" t="s">
         <v>90</v>
       </c>
       <c r="F76" t="s">
-        <v>107</v>
+        <v>110</v>
+      </c>
+      <c r="G76" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="C77" t="s">
         <v>88</v>
@@ -2363,15 +2381,15 @@
         <v>90</v>
       </c>
       <c r="F77" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C78" t="s">
         <v>87</v>
@@ -2385,19 +2403,16 @@
       <c r="F78" t="s">
         <v>110</v>
       </c>
-      <c r="G78" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="C79" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D79" t="s">
         <v>90</v>
@@ -2411,13 +2426,13 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C80" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D80" t="s">
         <v>90</v>
@@ -2431,10 +2446,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>80</v>
+        <v>94</v>
       </c>
       <c r="C81" t="s">
         <v>87</v>
@@ -2443,21 +2458,24 @@
         <v>90</v>
       </c>
       <c r="E81" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F81" t="s">
         <v>110</v>
       </c>
+      <c r="G81" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>81</v>
+        <v>10</v>
       </c>
       <c r="C82" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D82" t="s">
         <v>90</v>
@@ -2466,15 +2484,15 @@
         <v>90</v>
       </c>
       <c r="F82" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>82</v>
+        <v>40</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>94</v>
+        <v>40</v>
       </c>
       <c r="C83" t="s">
         <v>87</v>
@@ -2483,85 +2501,79 @@
         <v>90</v>
       </c>
       <c r="E83" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F83" t="s">
-        <v>110</v>
-      </c>
-      <c r="G83" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>83</v>
+        <v>41</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
       <c r="C84" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D84" t="s">
         <v>90</v>
       </c>
       <c r="E84" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F84" t="s">
-        <v>102</v>
-      </c>
-      <c r="G84" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>84</v>
-      </c>
-      <c r="B85" t="s">
-        <v>96</v>
+        <v>42</v>
+      </c>
+      <c r="B85" s="1" t="s">
+        <v>42</v>
       </c>
       <c r="C85" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D85" t="s">
         <v>90</v>
       </c>
       <c r="E85" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F85" t="s">
-        <v>98</v>
-      </c>
-      <c r="G85" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>85</v>
-      </c>
-      <c r="B86" t="s">
-        <v>97</v>
+        <v>43</v>
+      </c>
+      <c r="B86" s="1" t="s">
+        <v>43</v>
       </c>
       <c r="C86" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D86" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E86" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F86" t="s">
-        <v>101</v>
-      </c>
-      <c r="G86" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:G86" xr:uid="{6A589D3F-1078-EC4A-BFED-84F931FC0F8A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G86">
+      <sortCondition ref="F1:F86"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated working file and House_Variables file based on progress made.
</commit_message>
<xml_diff>
--- a/House_Variables.xlsx
+++ b/House_Variables.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nfaupel/Desktop/Projects/Housing_Price_Prediction/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80071DCC-4D3E-AB46-BF93-F70AC1917356}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75DC9ADB-62A1-1643-A885-A8B9903C6630}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1440" yWindow="1740" windowWidth="27640" windowHeight="16940" xr2:uid="{6CC0573A-78B8-8B47-B289-8880F04E05D3}"/>
+    <workbookView xWindow="-1000" yWindow="-20660" windowWidth="29020" windowHeight="18280" xr2:uid="{6CC0573A-78B8-8B47-B289-8880F04E05D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$86</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$88</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="457" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="475" uniqueCount="113">
   <si>
     <t>Column</t>
   </si>
@@ -372,6 +372,12 @@
   </si>
   <si>
     <t>sale detail</t>
+  </si>
+  <si>
+    <t>BsmtFinSF</t>
+  </si>
+  <si>
+    <t>BsmtFinished</t>
   </si>
 </sst>
 </file>
@@ -751,11 +757,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A589D3F-1078-EC4A-BFED-84F931FC0F8A}">
-  <dimension ref="A1:G86"/>
+  <dimension ref="A1:G88"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -874,6 +880,9 @@
       <c r="F5" t="s">
         <v>104</v>
       </c>
+      <c r="G5" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6">
@@ -894,6 +903,9 @@
       <c r="F6" t="s">
         <v>104</v>
       </c>
+      <c r="G6" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A7">
@@ -960,6 +972,9 @@
       <c r="F9" t="s">
         <v>104</v>
       </c>
+      <c r="G9" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10">
@@ -1003,6 +1018,9 @@
       <c r="F11" t="s">
         <v>104</v>
       </c>
+      <c r="G11" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12">
@@ -1023,6 +1041,9 @@
       <c r="F12" t="s">
         <v>104</v>
       </c>
+      <c r="G12" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13">
@@ -1043,13 +1064,16 @@
       <c r="F13" t="s">
         <v>104</v>
       </c>
+      <c r="G13" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14">
-        <v>48</v>
+        <v>86</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>48</v>
+        <v>111</v>
       </c>
       <c r="C14" t="s">
         <v>88</v>
@@ -1058,38 +1082,44 @@
         <v>90</v>
       </c>
       <c r="E14" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F14" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="G14" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15">
-        <v>49</v>
+        <v>87</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>49</v>
+        <v>112</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D15" t="s">
         <v>90</v>
       </c>
       <c r="E15" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F15" t="s">
-        <v>106</v>
+        <v>104</v>
+      </c>
+      <c r="G15" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C16" t="s">
         <v>88</v>
@@ -1106,10 +1136,10 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" t="s">
         <v>88</v>
@@ -1126,13 +1156,13 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>2</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D18" t="s">
         <v>90</v>
@@ -1141,21 +1171,18 @@
         <v>90</v>
       </c>
       <c r="F18" t="s">
-        <v>98</v>
-      </c>
-      <c r="G18" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>3</v>
+        <v>51</v>
       </c>
       <c r="C19" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D19" t="s">
         <v>90</v>
@@ -1164,18 +1191,15 @@
         <v>90</v>
       </c>
       <c r="F19" t="s">
-        <v>98</v>
-      </c>
-      <c r="G19" t="s">
-        <v>90</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="C20" t="s">
         <v>87</v>
@@ -1195,10 +1219,10 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="C21" t="s">
         <v>87</v>
@@ -1218,10 +1242,10 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="C22" t="s">
         <v>87</v>
@@ -1235,13 +1259,16 @@
       <c r="F22" t="s">
         <v>98</v>
       </c>
+      <c r="G22" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
       <c r="C23" t="s">
         <v>87</v>
@@ -1255,13 +1282,16 @@
       <c r="F23" t="s">
         <v>98</v>
       </c>
+      <c r="G23" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C24" t="s">
         <v>87</v>
@@ -1278,10 +1308,10 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C25" t="s">
         <v>87</v>
@@ -1298,16 +1328,16 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A26">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
         <v>87</v>
       </c>
       <c r="D26" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E26" t="s">
         <v>90</v>
@@ -1318,16 +1348,16 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A27">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C27" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D27" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E27" t="s">
         <v>90</v>
@@ -1335,22 +1365,19 @@
       <c r="F27" t="s">
         <v>98</v>
       </c>
-      <c r="G27" t="s">
-        <v>90</v>
-      </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A28">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C28" t="s">
         <v>87</v>
       </c>
       <c r="D28" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E28" t="s">
         <v>90</v>
@@ -1361,76 +1388,76 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A29">
-        <v>84</v>
-      </c>
-      <c r="B29" t="s">
-        <v>96</v>
+        <v>27</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="C29" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E29" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F29" t="s">
         <v>98</v>
       </c>
       <c r="G29" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A30">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>59</v>
+        <v>30</v>
       </c>
       <c r="C30" t="s">
         <v>87</v>
       </c>
       <c r="D30" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E30" t="s">
         <v>90</v>
       </c>
       <c r="F30" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A31">
-        <v>60</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>60</v>
+        <v>84</v>
+      </c>
+      <c r="B31" t="s">
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D31" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E31" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F31" t="s">
-        <v>108</v>
+        <v>98</v>
       </c>
       <c r="G31" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A32">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C32" t="s">
         <v>87</v>
@@ -1445,18 +1472,18 @@
         <v>108</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C33" t="s">
         <v>88</v>
       </c>
       <c r="D33" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E33" t="s">
         <v>90</v>
@@ -1464,19 +1491,22 @@
       <c r="F33" t="s">
         <v>108</v>
       </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="G33" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C34" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D34" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E34" t="s">
         <v>90</v>
@@ -1485,18 +1515,18 @@
         <v>108</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A35">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C35" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D35" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E35" t="s">
         <v>90</v>
@@ -1505,18 +1535,18 @@
         <v>108</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A36">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C36" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D36" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E36" t="s">
         <v>90</v>
@@ -1525,52 +1555,52 @@
         <v>108</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A37">
+        <v>64</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>87</v>
+      </c>
+      <c r="D37" t="s">
+        <v>85</v>
+      </c>
+      <c r="E37" t="s">
+        <v>90</v>
+      </c>
+      <c r="F37" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38">
+        <v>65</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
+        <v>85</v>
+      </c>
+      <c r="E38" t="s">
+        <v>90</v>
+      </c>
+      <c r="F38" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39">
         <v>18</v>
       </c>
-      <c r="B37" s="1" t="s">
+      <c r="B39" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="C37" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" t="s">
-        <v>90</v>
-      </c>
-      <c r="E37" t="s">
-        <v>90</v>
-      </c>
-      <c r="F37" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A38">
-        <v>19</v>
-      </c>
-      <c r="B38" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" t="s">
-        <v>87</v>
-      </c>
-      <c r="D38" t="s">
-        <v>90</v>
-      </c>
-      <c r="E38" t="s">
-        <v>90</v>
-      </c>
-      <c r="F38" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A39">
-        <v>28</v>
-      </c>
-      <c r="B39" s="1" t="s">
-        <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>87</v>
@@ -1585,12 +1615,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A40">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="C40" t="s">
         <v>87</v>
@@ -1605,12 +1635,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A41">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>54</v>
+        <v>28</v>
       </c>
       <c r="C41" t="s">
         <v>87</v>
@@ -1625,12 +1655,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A42">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="C42" t="s">
         <v>87</v>
@@ -1645,52 +1675,52 @@
         <v>103</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A43">
+        <v>54</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C43" t="s">
+        <v>87</v>
+      </c>
+      <c r="D43" t="s">
+        <v>90</v>
+      </c>
+      <c r="E43" t="s">
+        <v>90</v>
+      </c>
+      <c r="F43" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>56</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C44" t="s">
+        <v>87</v>
+      </c>
+      <c r="D44" t="s">
+        <v>90</v>
+      </c>
+      <c r="E44" t="s">
+        <v>90</v>
+      </c>
+      <c r="F44" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A45">
         <v>44</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="B45" s="1" t="s">
         <v>44</v>
-      </c>
-      <c r="C43" t="s">
-        <v>88</v>
-      </c>
-      <c r="D43" t="s">
-        <v>90</v>
-      </c>
-      <c r="E43" t="s">
-        <v>90</v>
-      </c>
-      <c r="F43" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A44">
-        <v>45</v>
-      </c>
-      <c r="B44" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="C44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D44" t="s">
-        <v>90</v>
-      </c>
-      <c r="E44" t="s">
-        <v>90</v>
-      </c>
-      <c r="F44" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45">
-        <v>46</v>
-      </c>
-      <c r="B45" s="1" t="s">
-        <v>46</v>
       </c>
       <c r="C45" t="s">
         <v>88</v>
@@ -1705,12 +1735,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A46">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C46" t="s">
         <v>88</v>
@@ -1725,12 +1755,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A47">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C47" t="s">
         <v>88</v>
@@ -1745,12 +1775,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A48">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C48" t="s">
         <v>88</v>
@@ -1767,10 +1797,10 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A49">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="C49" t="s">
         <v>88</v>
@@ -1787,13 +1817,13 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A50">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>1</v>
+        <v>53</v>
       </c>
       <c r="C50" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="D50" t="s">
         <v>90</v>
@@ -1802,21 +1832,18 @@
         <v>90</v>
       </c>
       <c r="F50" t="s">
-        <v>86</v>
-      </c>
-      <c r="G50" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A51">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>13</v>
+        <v>55</v>
       </c>
       <c r="C51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D51" t="s">
         <v>90</v>
@@ -1825,73 +1852,70 @@
         <v>90</v>
       </c>
       <c r="F51" t="s">
-        <v>101</v>
+        <v>105</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A52">
-        <v>85</v>
-      </c>
-      <c r="B52" t="s">
-        <v>97</v>
+        <v>1</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="D52" t="s">
         <v>90</v>
       </c>
       <c r="E52" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F52" t="s">
-        <v>101</v>
+        <v>86</v>
       </c>
       <c r="G52" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A53">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>4</v>
+        <v>13</v>
       </c>
       <c r="C53" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D53" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E53" t="s">
         <v>90</v>
       </c>
       <c r="F53" t="s">
-        <v>99</v>
-      </c>
-      <c r="G53" t="s">
-        <v>85</v>
+        <v>101</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A54">
-        <v>5</v>
-      </c>
-      <c r="B54" s="1" t="s">
-        <v>5</v>
+        <v>85</v>
+      </c>
+      <c r="B54" t="s">
+        <v>97</v>
       </c>
       <c r="C54" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D54" t="s">
         <v>90</v>
       </c>
       <c r="E54" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F54" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="G54" t="s">
         <v>85</v>
@@ -1899,16 +1923,16 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A55">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C55" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D55" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E55" t="s">
         <v>90</v>
@@ -1917,21 +1941,21 @@
         <v>99</v>
       </c>
       <c r="G55" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A56">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C56" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D56" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E56" t="s">
         <v>90</v>
@@ -1940,15 +1964,15 @@
         <v>99</v>
       </c>
       <c r="G56" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A57">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C57" t="s">
         <v>87</v>
@@ -1968,16 +1992,16 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A58">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C58" t="s">
         <v>87</v>
       </c>
       <c r="D58" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E58" t="s">
         <v>90</v>
@@ -1991,10 +2015,10 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A59">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C59" t="s">
         <v>87</v>
@@ -2014,10 +2038,10 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A60">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C60" t="s">
         <v>87</v>
@@ -2037,10 +2061,10 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A61">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C61" t="s">
         <v>87</v>
@@ -2060,10 +2084,10 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A62">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C62" t="s">
         <v>87</v>
@@ -2083,13 +2107,13 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A63">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>57</v>
+        <v>14</v>
       </c>
       <c r="C63" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D63" t="s">
         <v>90</v>
@@ -2098,38 +2122,44 @@
         <v>90</v>
       </c>
       <c r="F63" t="s">
-        <v>107</v>
+        <v>99</v>
+      </c>
+      <c r="G63" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A64">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>58</v>
+        <v>15</v>
       </c>
       <c r="C64" t="s">
         <v>87</v>
       </c>
       <c r="D64" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E64" t="s">
         <v>90</v>
       </c>
       <c r="F64" t="s">
-        <v>107</v>
+        <v>99</v>
+      </c>
+      <c r="G64" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A65">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C65" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D65" t="s">
         <v>90</v>
@@ -2143,16 +2173,16 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A66">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>72</v>
+        <v>58</v>
       </c>
       <c r="C66" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D66" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E66" t="s">
         <v>90</v>
@@ -2163,16 +2193,16 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A67">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
       <c r="C67" t="s">
         <v>87</v>
       </c>
       <c r="D67" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E67" t="s">
         <v>90</v>
@@ -2183,16 +2213,16 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A68">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C68" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D68" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E68" t="s">
         <v>90</v>
@@ -2203,16 +2233,16 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A69">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C69" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D69" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E69" t="s">
         <v>90</v>
@@ -2223,30 +2253,30 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A70">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C70" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D70" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E70" t="s">
         <v>90</v>
       </c>
       <c r="F70" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A71">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="C71" t="s">
         <v>88</v>
@@ -2258,15 +2288,15 @@
         <v>90</v>
       </c>
       <c r="F71" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A72">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C72" t="s">
         <v>88</v>
@@ -2283,10 +2313,10 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A73">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C73" t="s">
         <v>88</v>
@@ -2303,10 +2333,10 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A74">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
         <v>88</v>
@@ -2323,16 +2353,16 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A75">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D75" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E75" t="s">
         <v>90</v>
@@ -2343,13 +2373,13 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A76">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D76" t="s">
         <v>90</v>
@@ -2358,38 +2388,35 @@
         <v>90</v>
       </c>
       <c r="F76" t="s">
-        <v>110</v>
-      </c>
-      <c r="G76" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A77">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="C77" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D77" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="E77" t="s">
         <v>90</v>
       </c>
       <c r="F77" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A78">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C78" t="s">
         <v>87</v>
@@ -2403,16 +2430,19 @@
       <c r="F78" t="s">
         <v>110</v>
       </c>
+      <c r="G78" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A79">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C79" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D79" t="s">
         <v>90</v>
@@ -2426,13 +2456,13 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A80">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C80" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D80" t="s">
         <v>90</v>
@@ -2446,10 +2476,10 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A81">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>94</v>
+        <v>80</v>
       </c>
       <c r="C81" t="s">
         <v>87</v>
@@ -2458,24 +2488,21 @@
         <v>90</v>
       </c>
       <c r="E81" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="F81" t="s">
         <v>110</v>
       </c>
-      <c r="G81" t="s">
-        <v>85</v>
-      </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A82">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="C82" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D82" t="s">
         <v>90</v>
@@ -2484,15 +2511,15 @@
         <v>90</v>
       </c>
       <c r="F82" t="s">
-        <v>100</v>
+        <v>110</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A83">
-        <v>40</v>
+        <v>82</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>40</v>
+        <v>94</v>
       </c>
       <c r="C83" t="s">
         <v>87</v>
@@ -2501,18 +2528,21 @@
         <v>90</v>
       </c>
       <c r="E83" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="F83" t="s">
-        <v>100</v>
+        <v>110</v>
+      </c>
+      <c r="G83" t="s">
+        <v>85</v>
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A84">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C84" t="s">
         <v>87</v>
@@ -2529,13 +2559,13 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A85">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C85" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D85" t="s">
         <v>90</v>
@@ -2549,16 +2579,16 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A86">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C86" t="s">
         <v>87</v>
       </c>
       <c r="D86" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="E86" t="s">
         <v>90</v>
@@ -2567,10 +2597,50 @@
         <v>100</v>
       </c>
     </row>
+    <row r="87" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A87">
+        <v>42</v>
+      </c>
+      <c r="B87" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C87" t="s">
+        <v>89</v>
+      </c>
+      <c r="D87" t="s">
+        <v>90</v>
+      </c>
+      <c r="E87" t="s">
+        <v>90</v>
+      </c>
+      <c r="F87" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A88">
+        <v>43</v>
+      </c>
+      <c r="B88" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C88" t="s">
+        <v>87</v>
+      </c>
+      <c r="D88" t="s">
+        <v>85</v>
+      </c>
+      <c r="E88" t="s">
+        <v>90</v>
+      </c>
+      <c r="F88" t="s">
+        <v>100</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:G86" xr:uid="{6A589D3F-1078-EC4A-BFED-84F931FC0F8A}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G86">
-      <sortCondition ref="F1:F86"/>
+  <autoFilter ref="A1:G88" xr:uid="{6A589D3F-1078-EC4A-BFED-84F931FC0F8A}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:G88">
+      <sortCondition ref="F1:F88"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>